<commit_message>
Moved speed function to new file, added motor calibration
</commit_message>
<xml_diff>
--- a/motor_calibration.xlsx
+++ b/motor_calibration.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\James\Documents\GitHub\two-wheel-robot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CA84271-BE1E-4D96-9879-491E81AF82A5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0A2E242-E292-4218-82D6-FDD9BBC10F6E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{1D31DF6B-69DC-4335-9917-AC64ABE7BC70}"/>
+    <workbookView xWindow="20745" yWindow="4200" windowWidth="28800" windowHeight="15435" activeTab="1" xr2:uid="{1D31DF6B-69DC-4335-9917-AC64ABE7BC70}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -57,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Motor 1 +</t>
   </si>
@@ -87,6 +87,12 @@
   </si>
   <si>
     <t>Hz</t>
+  </si>
+  <si>
+    <t>f</t>
+  </si>
+  <si>
+    <t>v</t>
   </si>
 </sst>
 </file>
@@ -5366,8 +5372,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B94C1634-680D-4D95-89C4-8751F074763F}">
   <dimension ref="A3:Z35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="U33" sqref="U33"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5656,18 +5662,291 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86FB0BEC-8C00-4596-85BD-1C5CCDCE1CE6}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B30"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:B1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <f>(A2-Sheet1!T$32)/Sheet1!T$31</f>
+        <v>0.5016484418863143</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>100</v>
+      </c>
+      <c r="B3">
+        <f>(A3-Sheet1!T$32)/Sheet1!T$31</f>
+        <v>0.69856619125629638</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>200</v>
+      </c>
+      <c r="B4">
+        <f>(A4-Sheet1!T$32)/Sheet1!T$31</f>
+        <v>0.89548394062627856</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>300</v>
+      </c>
+      <c r="B5">
+        <f>(A5-Sheet1!T$32)/Sheet1!T$31</f>
+        <v>1.0924016899962605</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>400</v>
+      </c>
+      <c r="B6">
+        <f>(A6-Sheet1!T$32)/Sheet1!T$31</f>
+        <v>1.2893194393662426</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>500</v>
+      </c>
+      <c r="B7">
+        <f>(A7-Sheet1!T$32)/Sheet1!T$31</f>
+        <v>1.4862371887362247</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>600</v>
+      </c>
+      <c r="B8">
+        <f>(A8-Sheet1!T$32)/Sheet1!T$31</f>
+        <v>1.683154938106207</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>700</v>
+      </c>
+      <c r="B9">
+        <f>(A9-Sheet1!T$32)/Sheet1!T$31</f>
+        <v>1.8800726874761891</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>800</v>
+      </c>
+      <c r="B10">
+        <f>(A10-Sheet1!T$32)/Sheet1!T$31</f>
+        <v>2.0769904368461711</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>900</v>
+      </c>
+      <c r="B11">
+        <f>(A11-Sheet1!T$32)/Sheet1!T$31</f>
+        <v>2.2739081862161532</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>1000</v>
+      </c>
+      <c r="B12">
+        <f>(A12-Sheet1!T$32)/Sheet1!T$31</f>
+        <v>2.4708259355861353</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>1100</v>
+      </c>
+      <c r="B13">
+        <f>(A13-Sheet1!T$32)/Sheet1!T$31</f>
+        <v>2.6677436849561174</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>1200</v>
+      </c>
+      <c r="B14">
+        <f>(A14-Sheet1!T$32)/Sheet1!T$31</f>
+        <v>2.8646614343260994</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>1300</v>
+      </c>
+      <c r="B15">
+        <f>(A15-Sheet1!T$32)/Sheet1!T$31</f>
+        <v>3.0615791836960815</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>1400</v>
+      </c>
+      <c r="B16">
+        <f>(A16-Sheet1!T$32)/Sheet1!T$31</f>
+        <v>3.2584969330660636</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>1500</v>
+      </c>
+      <c r="B17">
+        <f>(A17-Sheet1!T$32)/Sheet1!T$31</f>
+        <v>3.4554146824360457</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>1600</v>
+      </c>
+      <c r="B18">
+        <f>(A18-Sheet1!T$32)/Sheet1!T$31</f>
+        <v>3.6523324318060277</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>1700</v>
+      </c>
+      <c r="B19">
+        <f>(A19-Sheet1!T$32)/Sheet1!T$31</f>
+        <v>3.8492501811760098</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>1800</v>
+      </c>
+      <c r="B20">
+        <f>(A20-Sheet1!T$32)/Sheet1!T$31</f>
+        <v>4.0461679305459919</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>1900</v>
+      </c>
+      <c r="B21">
+        <f>(A21-Sheet1!T$32)/Sheet1!T$31</f>
+        <v>4.243085679915974</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>2000</v>
+      </c>
+      <c r="B22">
+        <f>(A22-Sheet1!T$32)/Sheet1!T$31</f>
+        <v>4.440003429285956</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>2100</v>
+      </c>
+      <c r="B23">
+        <f>(A23-Sheet1!T$32)/Sheet1!T$31</f>
+        <v>4.6369211786559381</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>2200</v>
+      </c>
+      <c r="B24">
+        <f>(A24-Sheet1!T$32)/Sheet1!T$31</f>
+        <v>4.8338389280259202</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>2300</v>
+      </c>
+      <c r="B25">
+        <f>(A25-Sheet1!T$32)/Sheet1!T$31</f>
+        <v>5.0307566773959023</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>2400</v>
+      </c>
+      <c r="B26">
+        <f>(A26-Sheet1!T$32)/Sheet1!T$31</f>
+        <v>5.2276744267658843</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>2500</v>
+      </c>
+      <c r="B27">
+        <f>(A27-Sheet1!T$32)/Sheet1!T$31</f>
+        <v>5.4245921761358664</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>2600</v>
+      </c>
+      <c r="B28">
+        <f>(A28-Sheet1!T$32)/Sheet1!T$31</f>
+        <v>5.6215099255058485</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>2700</v>
+      </c>
+      <c r="B29">
+        <f>(A29-Sheet1!T$32)/Sheet1!T$31</f>
+        <v>5.8184276748758306</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>2800</v>
+      </c>
+      <c r="B30">
+        <f>(A30-Sheet1!T$32)/Sheet1!T$31</f>
+        <v>6.0153454242458126</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>